<commit_message>
Version 3.5; Made update for Arduino Gateway and fixed several smaller bugs
</commit_message>
<xml_diff>
--- a/transmitters/livolo/sniffer-livolo.xlsx
+++ b/transmitters/livolo/sniffer-livolo.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Blad4" sheetId="4" r:id="rId1"/>
@@ -15,8 +15,42 @@
   <definedNames>
     <definedName name="sniffer_livolo" localSheetId="0">Blad4!$B$1:$AK$222</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Auteur</author>
+  </authors>
+  <commentList>
+    <comment ref="B221" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+StartBit</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
@@ -67,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="24">
   <si>
     <t>===========================================</t>
   </si>
@@ -131,12 +165,21 @@
   <si>
     <t>Normalized</t>
   </si>
+  <si>
+    <t>23 values</t>
+  </si>
+  <si>
+    <t>unit=8</t>
+  </si>
+  <si>
+    <t>Addr=</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,8 +195,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,6 +246,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -203,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -212,6 +274,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -221,6 +284,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -273,7 +339,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -308,7 +374,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -516,29 +582,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BV232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="A210" sqref="A210"/>
+    <sheetView tabSelected="1" topLeftCell="B211" workbookViewId="0">
+      <selection activeCell="AN224" sqref="AN224"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="3" width="4.88671875" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="3" width="4.85546875" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="30" width="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.21875" customWidth="1"/>
+    <col min="31" max="31" width="5.28515625" customWidth="1"/>
     <col min="32" max="37" width="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.77734375" customWidth="1"/>
-    <col min="40" max="40" width="5.6640625" customWidth="1"/>
-    <col min="41" max="41" width="5.88671875" customWidth="1"/>
-    <col min="42" max="42" width="6.33203125" customWidth="1"/>
-    <col min="43" max="43" width="5.77734375" customWidth="1"/>
+    <col min="39" max="39" width="7.28515625" customWidth="1"/>
+    <col min="40" max="40" width="9.5703125" customWidth="1"/>
+    <col min="41" max="41" width="5.85546875" customWidth="1"/>
+    <col min="42" max="42" width="6.28515625" customWidth="1"/>
+    <col min="43" max="43" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>595</v>
       </c>
@@ -648,7 +714,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>489</v>
       </c>
@@ -758,7 +824,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>490</v>
       </c>
@@ -868,7 +934,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>481</v>
       </c>
@@ -978,7 +1044,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>479</v>
       </c>
@@ -1085,7 +1151,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>481</v>
       </c>
@@ -1192,7 +1258,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>483</v>
       </c>
@@ -1299,7 +1365,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>504</v>
       </c>
@@ -1406,7 +1472,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>475</v>
       </c>
@@ -1516,7 +1582,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>477</v>
       </c>
@@ -1626,7 +1692,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>472</v>
       </c>
@@ -1736,7 +1802,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>475</v>
       </c>
@@ -1846,7 +1912,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>475</v>
       </c>
@@ -1956,7 +2022,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>474</v>
       </c>
@@ -2066,7 +2132,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>456</v>
       </c>
@@ -2176,7 +2242,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>486</v>
       </c>
@@ -2286,7 +2352,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>472</v>
       </c>
@@ -2396,7 +2462,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>475</v>
       </c>
@@ -2506,7 +2572,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>474</v>
       </c>
@@ -2613,7 +2679,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="22" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:74" x14ac:dyDescent="0.25">
       <c r="AM22">
         <v>476</v>
       </c>
@@ -2717,7 +2783,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="23" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>549</v>
       </c>
@@ -2827,7 +2893,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>477</v>
       </c>
@@ -2937,7 +3003,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>472</v>
       </c>
@@ -3038,7 +3104,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>495</v>
       </c>
@@ -3148,7 +3214,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>476</v>
       </c>
@@ -3258,7 +3324,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>477</v>
       </c>
@@ -3368,7 +3434,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="29" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>473</v>
       </c>
@@ -3478,7 +3544,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="30" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>473</v>
       </c>
@@ -3588,7 +3654,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="31" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>477</v>
       </c>
@@ -3698,7 +3764,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="2:74" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:74" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>471</v>
       </c>
@@ -3808,7 +3874,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="33" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>473</v>
       </c>
@@ -3918,7 +3984,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>467</v>
       </c>
@@ -4028,7 +4094,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="35" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>480</v>
       </c>
@@ -4138,7 +4204,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>472</v>
       </c>
@@ -4248,7 +4314,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>475</v>
       </c>
@@ -4358,7 +4424,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>470</v>
       </c>
@@ -4468,7 +4534,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>469</v>
       </c>
@@ -4578,7 +4644,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="40" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>469</v>
       </c>
@@ -4688,7 +4754,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>470</v>
       </c>
@@ -4798,7 +4864,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>469</v>
       </c>
@@ -4908,7 +4974,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>481</v>
       </c>
@@ -5018,7 +5084,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="44" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>477</v>
       </c>
@@ -5128,7 +5194,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>480</v>
       </c>
@@ -5238,7 +5304,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>475</v>
       </c>
@@ -5348,7 +5414,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="47" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>475</v>
       </c>
@@ -5458,7 +5524,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="48" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>477</v>
       </c>
@@ -5568,7 +5634,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="49" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>474</v>
       </c>
@@ -5678,7 +5744,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>473</v>
       </c>
@@ -5788,7 +5854,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>473</v>
       </c>
@@ -5898,7 +5964,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="52" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>475</v>
       </c>
@@ -6008,7 +6074,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>475</v>
       </c>
@@ -6118,7 +6184,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="54" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>478</v>
       </c>
@@ -6228,7 +6294,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="55" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>479</v>
       </c>
@@ -6338,7 +6404,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="56" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>473</v>
       </c>
@@ -6448,7 +6514,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="57" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>474</v>
       </c>
@@ -6558,7 +6624,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="58" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>474</v>
       </c>
@@ -6668,7 +6734,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="59" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>476</v>
       </c>
@@ -6778,7 +6844,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="60" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>473</v>
       </c>
@@ -6888,7 +6954,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="61" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>475</v>
       </c>
@@ -6998,7 +7064,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="62" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>475</v>
       </c>
@@ -7108,7 +7174,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="63" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>477</v>
       </c>
@@ -7218,7 +7284,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="64" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>474</v>
       </c>
@@ -7328,7 +7394,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="65" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>480</v>
       </c>
@@ -7438,7 +7504,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="66" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>469</v>
       </c>
@@ -7548,7 +7614,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>477</v>
       </c>
@@ -7658,7 +7724,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="68" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>472</v>
       </c>
@@ -7768,7 +7834,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="69" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>481</v>
       </c>
@@ -7878,7 +7944,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="70" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>475</v>
       </c>
@@ -7988,7 +8054,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="71" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>472</v>
       </c>
@@ -8098,7 +8164,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="72" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>475</v>
       </c>
@@ -8208,7 +8274,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="73" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>476</v>
       </c>
@@ -8318,7 +8384,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="74" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>473</v>
       </c>
@@ -8428,7 +8494,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="75" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>486</v>
       </c>
@@ -8538,7 +8604,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="76" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>488</v>
       </c>
@@ -8648,7 +8714,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>485</v>
       </c>
@@ -8758,7 +8824,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="78" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>488</v>
       </c>
@@ -8868,7 +8934,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="79" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>483</v>
       </c>
@@ -8978,7 +9044,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>485</v>
       </c>
@@ -9088,7 +9154,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="81" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>486</v>
       </c>
@@ -9198,7 +9264,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="82" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>488</v>
       </c>
@@ -9308,7 +9374,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="83" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>487</v>
       </c>
@@ -9418,7 +9484,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="84" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>484</v>
       </c>
@@ -9528,7 +9594,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="85" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>494</v>
       </c>
@@ -9638,7 +9704,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>485</v>
       </c>
@@ -9748,7 +9814,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="87" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>488</v>
       </c>
@@ -9858,7 +9924,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="88" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>488</v>
       </c>
@@ -9968,7 +10034,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="89" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>484</v>
       </c>
@@ -10078,7 +10144,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="90" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>487</v>
       </c>
@@ -10188,7 +10254,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="91" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>492</v>
       </c>
@@ -10298,7 +10364,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="92" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>487</v>
       </c>
@@ -10408,7 +10474,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="93" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>485</v>
       </c>
@@ -10518,7 +10584,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="94" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>486</v>
       </c>
@@ -10628,7 +10694,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="95" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>490</v>
       </c>
@@ -10738,7 +10804,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>526</v>
       </c>
@@ -10848,7 +10914,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>493</v>
       </c>
@@ -10958,7 +11024,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="98" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>486</v>
       </c>
@@ -11068,7 +11134,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="99" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>484</v>
       </c>
@@ -11178,7 +11244,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="100" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>485</v>
       </c>
@@ -11288,7 +11354,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="101" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>494</v>
       </c>
@@ -11398,7 +11464,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="102" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>486</v>
       </c>
@@ -11508,7 +11574,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="103" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>486</v>
       </c>
@@ -11618,7 +11684,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="104" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>485</v>
       </c>
@@ -11728,7 +11794,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="105" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>488</v>
       </c>
@@ -11838,7 +11904,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="106" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>484</v>
       </c>
@@ -11948,7 +12014,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="107" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>500</v>
       </c>
@@ -12058,7 +12124,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="108" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>478</v>
       </c>
@@ -12168,7 +12234,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="109" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>487</v>
       </c>
@@ -12278,7 +12344,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="110" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>484</v>
       </c>
@@ -12388,7 +12454,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="111" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>482</v>
       </c>
@@ -12498,7 +12564,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="113" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>2</v>
       </c>
@@ -12647,7 +12713,7 @@
         <v>188.25471698113208</v>
       </c>
     </row>
-    <row r="114" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>7</v>
       </c>
@@ -12760,7 +12826,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="115" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>3</v>
       </c>
@@ -12870,7 +12936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C116">
         <f>C113-C114</f>
         <v>73.879629629629619</v>
@@ -12944,7 +13010,7 @@
         <v>78.254716981132077</v>
       </c>
     </row>
-    <row r="117" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B117">
         <f>B113-B114</f>
         <v>-18.203703703703695</v>
@@ -13018,12 +13084,12 @@
         <v>12.896226415094333</v>
       </c>
     </row>
-    <row r="119" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>638</v>
       </c>
@@ -13133,7 +13199,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="122" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>485</v>
       </c>
@@ -13243,7 +13309,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="123" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>522</v>
       </c>
@@ -13353,7 +13419,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="124" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>510</v>
       </c>
@@ -13463,7 +13529,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="125" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>484</v>
       </c>
@@ -13573,7 +13639,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="126" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>481</v>
       </c>
@@ -13683,7 +13749,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="127" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B127">
         <v>485</v>
       </c>
@@ -13793,7 +13859,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="128" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B128">
         <v>483</v>
       </c>
@@ -13903,7 +13969,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="129" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B129">
         <v>482</v>
       </c>
@@ -14013,7 +14079,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="130" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B130">
         <v>478</v>
       </c>
@@ -14123,7 +14189,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="131" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B131">
         <v>479</v>
       </c>
@@ -14233,7 +14299,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="132" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B132">
         <v>479</v>
       </c>
@@ -14343,7 +14409,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="133" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B133">
         <v>482</v>
       </c>
@@ -14453,7 +14519,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="134" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B134">
         <v>473</v>
       </c>
@@ -14563,7 +14629,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="135" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B135">
         <v>477</v>
       </c>
@@ -14673,7 +14739,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="136" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B136">
         <v>476</v>
       </c>
@@ -14783,7 +14849,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="137" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B137">
         <v>479</v>
       </c>
@@ -14893,7 +14959,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="138" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B138">
         <v>476</v>
       </c>
@@ -15003,7 +15069,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="139" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B139">
         <v>468</v>
       </c>
@@ -15113,7 +15179,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="140" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B140">
         <v>441</v>
       </c>
@@ -15223,7 +15289,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="141" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B141">
         <v>476</v>
       </c>
@@ -15333,7 +15399,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="142" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B142">
         <v>476</v>
       </c>
@@ -15443,7 +15509,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="143" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B143">
         <v>477</v>
       </c>
@@ -15553,7 +15619,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="144" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B144">
         <v>476</v>
       </c>
@@ -15663,7 +15729,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="145" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B145">
         <v>471</v>
       </c>
@@ -15773,7 +15839,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="146" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B146">
         <v>472</v>
       </c>
@@ -15883,7 +15949,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B147">
         <v>477</v>
       </c>
@@ -15993,7 +16059,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="148" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B148">
         <v>480</v>
       </c>
@@ -16103,7 +16169,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="149" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B149">
         <v>475</v>
       </c>
@@ -16213,7 +16279,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="150" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B150">
         <v>478</v>
       </c>
@@ -16323,7 +16389,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="151" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B151">
         <v>474</v>
       </c>
@@ -16433,7 +16499,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="152" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B152">
         <v>473</v>
       </c>
@@ -16543,7 +16609,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="153" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B153">
         <v>477</v>
       </c>
@@ -16653,7 +16719,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="154" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B154">
         <v>472</v>
       </c>
@@ -16763,7 +16829,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="155" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B155">
         <v>480</v>
       </c>
@@ -16873,7 +16939,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="156" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B156">
         <v>473</v>
       </c>
@@ -16983,7 +17049,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="157" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B157">
         <v>469</v>
       </c>
@@ -17093,7 +17159,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="158" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B158">
         <v>475</v>
       </c>
@@ -17203,7 +17269,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="159" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B159">
         <v>473</v>
       </c>
@@ -17313,7 +17379,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="160" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B160">
         <v>474</v>
       </c>
@@ -17423,7 +17489,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="161" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B161">
         <v>469</v>
       </c>
@@ -17533,7 +17599,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="162" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B162">
         <v>473</v>
       </c>
@@ -17643,7 +17709,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="163" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B163">
         <v>473</v>
       </c>
@@ -17753,7 +17819,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="164" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B164">
         <v>474</v>
       </c>
@@ -17863,7 +17929,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="165" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B165">
         <v>473</v>
       </c>
@@ -17973,7 +18039,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="166" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B166">
         <v>474</v>
       </c>
@@ -18083,7 +18149,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="167" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B167">
         <v>471</v>
       </c>
@@ -18193,7 +18259,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="168" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B168">
         <v>472</v>
       </c>
@@ -18303,7 +18369,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="169" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B169">
         <v>470</v>
       </c>
@@ -18413,7 +18479,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="170" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B170">
         <v>470</v>
       </c>
@@ -18523,7 +18589,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="171" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B171">
         <v>467</v>
       </c>
@@ -18633,7 +18699,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="172" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B172">
         <v>492</v>
       </c>
@@ -18743,7 +18809,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="173" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B173">
         <v>497</v>
       </c>
@@ -18853,7 +18919,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="174" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B174">
         <v>483</v>
       </c>
@@ -18963,7 +19029,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="175" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B175">
         <v>487</v>
       </c>
@@ -19073,7 +19139,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="176" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B176">
         <v>485</v>
       </c>
@@ -19183,7 +19249,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="177" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B177">
         <v>488</v>
       </c>
@@ -19293,7 +19359,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="178" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B178">
         <v>485</v>
       </c>
@@ -19403,7 +19469,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="179" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B179">
         <v>482</v>
       </c>
@@ -19513,7 +19579,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="180" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B180">
         <v>482</v>
       </c>
@@ -19623,7 +19689,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="181" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B181">
         <v>484</v>
       </c>
@@ -19733,7 +19799,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="182" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B182">
         <v>482</v>
       </c>
@@ -19843,7 +19909,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="183" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B183">
         <v>453</v>
       </c>
@@ -19953,7 +20019,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="184" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B184">
         <v>483</v>
       </c>
@@ -20063,7 +20129,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="185" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B185">
         <v>483</v>
       </c>
@@ -20173,7 +20239,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="186" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B186">
         <v>482</v>
       </c>
@@ -20283,7 +20349,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="187" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B187">
         <v>483</v>
       </c>
@@ -20393,7 +20459,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="188" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B188">
         <v>477</v>
       </c>
@@ -20503,7 +20569,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="189" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B189">
         <v>471</v>
       </c>
@@ -20613,7 +20679,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="190" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B190">
         <v>471</v>
       </c>
@@ -20723,7 +20789,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="191" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B191">
         <v>470</v>
       </c>
@@ -20833,7 +20899,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="192" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B192">
         <v>470</v>
       </c>
@@ -20943,7 +21009,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="193" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B193">
         <v>469</v>
       </c>
@@ -21053,7 +21119,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="194" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B194">
         <v>471</v>
       </c>
@@ -21163,7 +21229,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="195" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B195">
         <v>468</v>
       </c>
@@ -21273,7 +21339,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="196" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B196">
         <v>470</v>
       </c>
@@ -21383,7 +21449,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B197">
         <v>474</v>
       </c>
@@ -21493,7 +21559,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="198" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B198">
         <v>475</v>
       </c>
@@ -21603,7 +21669,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="199" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B199">
         <v>469</v>
       </c>
@@ -21713,7 +21779,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="200" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B200">
         <v>471</v>
       </c>
@@ -21823,7 +21889,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="201" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B201">
         <v>470</v>
       </c>
@@ -21933,7 +21999,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="202" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B202">
         <v>471</v>
       </c>
@@ -22043,7 +22109,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="203" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B203">
         <v>470</v>
       </c>
@@ -22153,7 +22219,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="204" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B204">
         <v>471</v>
       </c>
@@ -22263,7 +22329,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="205" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B205">
         <v>470</v>
       </c>
@@ -22373,7 +22439,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="206" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B206">
         <v>470</v>
       </c>
@@ -22483,7 +22549,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="207" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B207">
         <v>469</v>
       </c>
@@ -22593,7 +22659,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="208" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B208">
         <v>475</v>
       </c>
@@ -22703,7 +22769,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="209" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B209">
         <v>476</v>
       </c>
@@ -22813,7 +22879,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="210" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B210">
         <v>470</v>
       </c>
@@ -22923,7 +22989,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="211" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B211">
         <v>470</v>
       </c>
@@ -23033,7 +23099,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="212" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B212">
         <v>467</v>
       </c>
@@ -23143,7 +23209,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="213" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B213">
         <v>469</v>
       </c>
@@ -23253,7 +23319,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="214" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B214">
         <v>473</v>
       </c>
@@ -23363,7 +23429,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="215" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B215">
         <v>468</v>
       </c>
@@ -23473,7 +23539,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="216" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B216">
         <v>469</v>
       </c>
@@ -23583,7 +23649,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="218" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B218" s="2">
         <f>AVERAGE(B122:B216)</f>
         <v>475.88421052631577</v>
@@ -23593,7 +23659,7 @@
         <v>189.33333333333334</v>
       </c>
       <c r="D218" s="3">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D121:D217)</f>
         <v>119.94736842105263</v>
       </c>
       <c r="E218" s="5">
@@ -23729,45 +23795,100 @@
         <v>191.34375</v>
       </c>
     </row>
-    <row r="219" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B219" s="2"/>
       <c r="C219" s="3"/>
-      <c r="D219" s="3"/>
-      <c r="E219" s="5"/>
+      <c r="D219" s="3">
+        <v>0</v>
+      </c>
+      <c r="E219" s="5">
+        <v>1</v>
+      </c>
       <c r="F219" s="3"/>
-      <c r="G219" s="3"/>
-      <c r="H219" s="5"/>
-      <c r="I219" s="5"/>
-      <c r="J219" s="5"/>
+      <c r="G219" s="3">
+        <v>0</v>
+      </c>
+      <c r="H219" s="5">
+        <v>1</v>
+      </c>
+      <c r="I219" s="5">
+        <v>1</v>
+      </c>
+      <c r="J219" s="5">
+        <v>1</v>
+      </c>
       <c r="K219" s="3"/>
-      <c r="L219" s="3"/>
+      <c r="L219" s="3">
+        <v>0</v>
+      </c>
       <c r="M219" s="4"/>
-      <c r="N219" s="4"/>
-      <c r="O219" s="5"/>
-      <c r="P219" s="5"/>
-      <c r="Q219" s="5"/>
+      <c r="N219" s="4">
+        <v>0</v>
+      </c>
+      <c r="O219" s="5">
+        <v>1</v>
+      </c>
+      <c r="P219" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q219" s="5">
+        <v>1</v>
+      </c>
       <c r="R219" s="3"/>
-      <c r="S219" s="3"/>
+      <c r="S219" s="3">
+        <v>0</v>
+      </c>
       <c r="T219" s="4"/>
-      <c r="U219" s="4"/>
-      <c r="V219" s="5"/>
-      <c r="W219" s="5"/>
-      <c r="X219" s="5"/>
+      <c r="U219" s="4">
+        <v>0</v>
+      </c>
+      <c r="V219" s="5">
+        <v>1</v>
+      </c>
+      <c r="W219" s="5">
+        <v>1</v>
+      </c>
+      <c r="X219" s="5">
+        <v>1</v>
+      </c>
       <c r="Y219" s="3"/>
-      <c r="Z219" s="3"/>
+      <c r="Z219" s="3">
+        <v>0</v>
+      </c>
       <c r="AA219" s="4"/>
-      <c r="AB219" s="4"/>
+      <c r="AB219" s="4">
+        <v>0</v>
+      </c>
       <c r="AC219" s="3"/>
-      <c r="AD219" s="3"/>
-      <c r="AE219" s="5"/>
+      <c r="AD219" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE219" s="5">
+        <v>1</v>
+      </c>
       <c r="AF219" s="3"/>
-      <c r="AG219" s="3"/>
+      <c r="AG219" s="3">
+        <v>0</v>
+      </c>
       <c r="AH219" s="4"/>
-      <c r="AI219" s="4"/>
+      <c r="AI219" s="4">
+        <v>0</v>
+      </c>
       <c r="AJ219" s="3"/>
-      <c r="AK219" s="3"/>
+      <c r="AK219" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL219" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM219" t="s">
+        <v>23</v>
+      </c>
+      <c r="AN219" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="220" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>19</v>
       </c>
@@ -23839,11 +23960,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="221" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>20</v>
       </c>
-      <c r="B221">
+      <c r="B221" s="8">
         <v>500</v>
       </c>
       <c r="C221">
@@ -23952,7 +24073,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="222" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
         <v>12</v>
       </c>
@@ -24062,7 +24183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>5</v>
       </c>
@@ -24139,7 +24260,7 @@
         <v>81.34375</v>
       </c>
     </row>
-    <row r="224" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>6</v>
       </c>
@@ -24216,7 +24337,7 @@
         <v>9.6421052631579016</v>
       </c>
     </row>
-    <row r="226" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A226" s="7" t="s">
         <v>15</v>
       </c>
@@ -24293,7 +24414,7 @@
         <v>81.34375</v>
       </c>
     </row>
-    <row r="227" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A227" s="7" t="s">
         <v>16</v>
       </c>
@@ -24352,7 +24473,7 @@
       <c r="AJ227" s="7"/>
       <c r="AK227" s="7"/>
     </row>
-    <row r="228" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A228" s="7" t="s">
         <v>17</v>
       </c>
@@ -24429,7 +24550,7 @@
       </c>
       <c r="AK228" s="7"/>
     </row>
-    <row r="229" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A229" s="7" t="s">
         <v>18</v>
       </c>
@@ -24485,12 +24606,12 @@
       <c r="AJ229" s="7"/>
       <c r="AK229" s="7"/>
     </row>
-    <row r="231" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="232" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>8</v>
       </c>
@@ -24642,6 +24763,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -24653,7 +24775,7 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24665,7 +24787,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24677,7 +24799,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>